<commit_message>
parapapapa bang bang boom boom powpow
WOLLAH
</commit_message>
<xml_diff>
--- a/Algemeen/Assetlist 2.0.xlsx
+++ b/Algemeen/Assetlist 2.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1031,7 +1031,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1053,6 +1053,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1212,7 +1224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1250,6 +1262,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1566,8 +1580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F176" sqref="F176:J176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2547,6 +2561,9 @@
       <c r="C58" t="s">
         <v>52</v>
       </c>
+      <c r="F58" s="35"/>
+      <c r="H58" s="35"/>
+      <c r="J58" s="35"/>
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
     </row>
@@ -2557,6 +2574,9 @@
       <c r="C59" t="s">
         <v>53</v>
       </c>
+      <c r="F59" s="35"/>
+      <c r="H59" s="35"/>
+      <c r="J59" s="35"/>
       <c r="L59" s="6"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -2591,6 +2611,9 @@
         <v>58</v>
       </c>
       <c r="D62" s="1"/>
+      <c r="F62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="J62" s="26"/>
       <c r="L62" s="6"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -2600,6 +2623,9 @@
       <c r="C63" t="s">
         <v>56</v>
       </c>
+      <c r="F63" s="26"/>
+      <c r="H63" s="26"/>
+      <c r="J63" s="26"/>
       <c r="L63" s="6"/>
       <c r="O63" s="1"/>
     </row>
@@ -2625,11 +2651,11 @@
       </c>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
+      <c r="F65" s="26"/>
       <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
+      <c r="H65" s="26"/>
       <c r="I65" s="9"/>
-      <c r="J65" s="9"/>
+      <c r="J65" s="26"/>
       <c r="K65" s="9"/>
       <c r="L65" s="7"/>
     </row>
@@ -2736,6 +2762,9 @@
       <c r="C71" t="s">
         <v>70</v>
       </c>
+      <c r="F71" s="26"/>
+      <c r="H71" s="26"/>
+      <c r="J71" s="26"/>
       <c r="L71" s="6"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -2745,6 +2774,9 @@
       <c r="C72" t="s">
         <v>71</v>
       </c>
+      <c r="F72" s="26"/>
+      <c r="H72" s="26"/>
+      <c r="J72" s="26"/>
       <c r="L72" s="6"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
@@ -2754,6 +2786,9 @@
       <c r="C73" t="s">
         <v>72</v>
       </c>
+      <c r="F73" s="26"/>
+      <c r="H73" s="26"/>
+      <c r="J73" s="26"/>
       <c r="L73" s="6"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -2763,6 +2798,9 @@
       <c r="C74" t="s">
         <v>73</v>
       </c>
+      <c r="F74" s="26"/>
+      <c r="H74" s="26"/>
+      <c r="J74" s="26"/>
       <c r="L74" s="6"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -2772,6 +2810,9 @@
       <c r="C75" t="s">
         <v>74</v>
       </c>
+      <c r="F75" s="26"/>
+      <c r="H75" s="26"/>
+      <c r="J75" s="26"/>
       <c r="L75" s="6"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
@@ -2781,7 +2822,9 @@
       <c r="C76" t="s">
         <v>75</v>
       </c>
-      <c r="H76" s="27"/>
+      <c r="F76" s="26"/>
+      <c r="H76" s="26"/>
+      <c r="J76" s="26"/>
       <c r="L76" s="6"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
@@ -2791,7 +2834,9 @@
       <c r="C77" t="s">
         <v>76</v>
       </c>
-      <c r="H77" s="27"/>
+      <c r="F77" s="26"/>
+      <c r="H77" s="26"/>
+      <c r="J77" s="26"/>
       <c r="L77" s="6"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
@@ -2801,6 +2846,9 @@
       <c r="C78" t="s">
         <v>77</v>
       </c>
+      <c r="F78" s="26"/>
+      <c r="H78" s="26"/>
+      <c r="J78" s="26"/>
       <c r="L78" s="6"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
@@ -2880,6 +2928,9 @@
       <c r="C84" t="s">
         <v>88</v>
       </c>
+      <c r="F84" s="26"/>
+      <c r="H84" s="26"/>
+      <c r="J84" s="26"/>
       <c r="L84" s="6"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -2910,6 +2961,9 @@
       <c r="C87" t="s">
         <v>91</v>
       </c>
+      <c r="F87" s="26"/>
+      <c r="H87" s="26"/>
+      <c r="J87" s="26"/>
       <c r="L87" s="6"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -2952,6 +3006,7 @@
       <c r="C91" t="s">
         <v>95</v>
       </c>
+      <c r="H91" s="26"/>
       <c r="L91" s="6"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -3059,6 +3114,9 @@
       <c r="C99" t="s">
         <v>56</v>
       </c>
+      <c r="F99" s="26"/>
+      <c r="H99" s="26"/>
+      <c r="J99" s="26"/>
       <c r="L99" s="6"/>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
@@ -3068,6 +3126,9 @@
       <c r="C100" t="s">
         <v>110</v>
       </c>
+      <c r="F100" s="26"/>
+      <c r="H100" s="26"/>
+      <c r="J100" s="26"/>
       <c r="L100" s="6"/>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
@@ -3077,6 +3138,9 @@
       <c r="C101" t="s">
         <v>94</v>
       </c>
+      <c r="F101" s="26"/>
+      <c r="H101" s="26"/>
+      <c r="J101" s="26"/>
       <c r="L101" s="6"/>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
@@ -3110,7 +3174,9 @@
       <c r="C104" t="s">
         <v>113</v>
       </c>
+      <c r="F104" s="26"/>
       <c r="H104" s="26"/>
+      <c r="J104" s="26"/>
       <c r="L104" s="6"/>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
@@ -3120,6 +3186,9 @@
       <c r="C105" t="s">
         <v>114</v>
       </c>
+      <c r="F105" s="26"/>
+      <c r="H105" s="26"/>
+      <c r="J105" s="26"/>
       <c r="L105" s="6"/>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
@@ -3138,6 +3207,9 @@
       <c r="C107" t="s">
         <v>116</v>
       </c>
+      <c r="F107" s="26"/>
+      <c r="H107" s="26"/>
+      <c r="J107" s="26"/>
       <c r="L107" s="6"/>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
@@ -3147,6 +3219,9 @@
       <c r="C108" t="s">
         <v>117</v>
       </c>
+      <c r="F108" s="26"/>
+      <c r="H108" s="26"/>
+      <c r="J108" s="26"/>
       <c r="L108" s="6"/>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
@@ -3156,6 +3231,9 @@
       <c r="C109" t="s">
         <v>118</v>
       </c>
+      <c r="F109" s="26"/>
+      <c r="H109" s="26"/>
+      <c r="J109" s="26"/>
       <c r="L109" s="6"/>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
@@ -3165,6 +3243,9 @@
       <c r="C110" t="s">
         <v>119</v>
       </c>
+      <c r="F110" s="26"/>
+      <c r="H110" s="26"/>
+      <c r="J110" s="26"/>
       <c r="L110" s="6"/>
     </row>
     <row r="111" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3177,11 +3258,9 @@
       </c>
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
-      <c r="F111" s="29"/>
-      <c r="G111" s="29"/>
-      <c r="H111" s="27"/>
-      <c r="I111" s="7"/>
-      <c r="J111" s="29"/>
+      <c r="F111" s="26"/>
+      <c r="H111" s="26"/>
+      <c r="J111" s="26"/>
       <c r="K111" s="29"/>
       <c r="L111" s="29"/>
       <c r="M111" s="7"/>
@@ -3234,6 +3313,9 @@
       <c r="C114" s="8" t="s">
         <v>132</v>
       </c>
+      <c r="F114" s="26"/>
+      <c r="H114" s="26"/>
+      <c r="J114" s="26"/>
       <c r="L114" s="6"/>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
@@ -3243,6 +3325,9 @@
       <c r="C115" s="8" t="s">
         <v>117</v>
       </c>
+      <c r="F115" s="26"/>
+      <c r="H115" s="26"/>
+      <c r="J115" s="26"/>
       <c r="L115" s="6"/>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
@@ -3252,6 +3337,9 @@
       <c r="C116" s="8" t="s">
         <v>133</v>
       </c>
+      <c r="F116" s="26"/>
+      <c r="H116" s="26"/>
+      <c r="J116" s="26"/>
       <c r="L116" s="6"/>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
@@ -3280,6 +3368,9 @@
       <c r="C119" s="8" t="s">
         <v>95</v>
       </c>
+      <c r="F119" s="26"/>
+      <c r="H119" s="26"/>
+      <c r="J119" s="26"/>
       <c r="L119" s="6"/>
     </row>
     <row r="120" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3319,7 +3410,9 @@
       <c r="C121" s="8" t="s">
         <v>140</v>
       </c>
+      <c r="F121" s="26"/>
       <c r="H121" s="26"/>
+      <c r="J121" s="26"/>
       <c r="L121" s="6"/>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
@@ -3329,6 +3422,7 @@
       <c r="C122" s="8" t="s">
         <v>141</v>
       </c>
+      <c r="H122" s="26"/>
       <c r="L122" s="6"/>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.25">
@@ -3338,7 +3432,9 @@
       <c r="C123" s="8" t="s">
         <v>142</v>
       </c>
+      <c r="F123" s="26"/>
       <c r="H123" s="26"/>
+      <c r="J123" s="26"/>
       <c r="L123" s="6"/>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
@@ -3348,6 +3444,9 @@
       <c r="C124" s="8" t="s">
         <v>143</v>
       </c>
+      <c r="F124" s="26"/>
+      <c r="H124" s="26"/>
+      <c r="J124" s="26"/>
       <c r="L124" s="6"/>
     </row>
     <row r="125" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3430,6 +3529,9 @@
       <c r="C131" s="8" t="s">
         <v>119</v>
       </c>
+      <c r="F131" s="26"/>
+      <c r="H131" s="26"/>
+      <c r="J131" s="26"/>
       <c r="L131" s="6"/>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.25">
@@ -3494,7 +3596,9 @@
       <c r="C135" t="s">
         <v>98</v>
       </c>
-      <c r="H135" s="27"/>
+      <c r="F135" s="26"/>
+      <c r="H135" s="26"/>
+      <c r="J135" s="26"/>
       <c r="L135" s="6"/>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
@@ -3504,7 +3608,9 @@
       <c r="C136" t="s">
         <v>161</v>
       </c>
+      <c r="F136" s="26"/>
       <c r="H136" s="26"/>
+      <c r="J136" s="26"/>
       <c r="L136" s="6"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
@@ -3514,6 +3620,9 @@
       <c r="C137" t="s">
         <v>110</v>
       </c>
+      <c r="F137" s="26"/>
+      <c r="H137" s="26"/>
+      <c r="J137" s="26"/>
       <c r="L137" s="6"/>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
@@ -3523,6 +3632,9 @@
       <c r="C138" t="s">
         <v>162</v>
       </c>
+      <c r="F138" s="36"/>
+      <c r="H138" s="26"/>
+      <c r="J138" s="26"/>
       <c r="L138" s="6"/>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.25">
@@ -3532,6 +3644,9 @@
       <c r="C139" t="s">
         <v>165</v>
       </c>
+      <c r="F139" s="26"/>
+      <c r="H139" s="26"/>
+      <c r="J139" s="26"/>
       <c r="L139" s="6"/>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.25">
@@ -3559,7 +3674,9 @@
       <c r="C142" s="8" t="s">
         <v>132</v>
       </c>
+      <c r="F142" s="26"/>
       <c r="H142" s="26"/>
+      <c r="J142" s="26"/>
       <c r="L142" s="6"/>
     </row>
     <row r="143" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3606,6 +3723,9 @@
       <c r="C145" s="8" t="s">
         <v>110</v>
       </c>
+      <c r="F145" s="26"/>
+      <c r="H145" s="26"/>
+      <c r="J145" s="26"/>
       <c r="L145" s="6"/>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
@@ -3615,6 +3735,9 @@
       <c r="C146" s="8" t="s">
         <v>162</v>
       </c>
+      <c r="F146" s="26"/>
+      <c r="H146" s="26"/>
+      <c r="J146" s="26"/>
       <c r="L146" s="6"/>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
@@ -3624,6 +3747,9 @@
       <c r="C147" s="8" t="s">
         <v>117</v>
       </c>
+      <c r="F147" s="26"/>
+      <c r="H147" s="26"/>
+      <c r="J147" s="26"/>
       <c r="L147" s="6"/>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
@@ -3642,6 +3768,9 @@
       <c r="C149" s="8" t="s">
         <v>118</v>
       </c>
+      <c r="F149" s="26"/>
+      <c r="H149" s="26"/>
+      <c r="J149" s="26"/>
       <c r="L149" s="6"/>
     </row>
     <row r="150" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3707,6 +3836,9 @@
       <c r="C153" t="s">
         <v>117</v>
       </c>
+      <c r="F153" s="26"/>
+      <c r="H153" s="26"/>
+      <c r="J153" s="26"/>
       <c r="L153" s="6"/>
     </row>
     <row r="154" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3831,7 +3963,9 @@
       <c r="C162" s="10" t="s">
         <v>186</v>
       </c>
+      <c r="F162" s="26"/>
       <c r="H162" s="26"/>
+      <c r="J162" s="26"/>
       <c r="L162" s="6"/>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.25">
@@ -3841,7 +3975,9 @@
       <c r="C163" s="8" t="s">
         <v>191</v>
       </c>
+      <c r="F163" s="26"/>
       <c r="H163" s="26"/>
+      <c r="J163" s="26"/>
       <c r="L163" s="6"/>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
@@ -3851,6 +3987,9 @@
       <c r="C164" t="s">
         <v>165</v>
       </c>
+      <c r="F164" s="26"/>
+      <c r="H164" s="26"/>
+      <c r="J164" s="26"/>
       <c r="L164" s="6"/>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.25">
@@ -3925,7 +4064,9 @@
       <c r="C170" t="s">
         <v>252</v>
       </c>
-      <c r="H170" s="27"/>
+      <c r="F170" s="26"/>
+      <c r="H170" s="26"/>
+      <c r="J170" s="26"/>
       <c r="L170" s="6"/>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.25">
@@ -3935,7 +4076,7 @@
       <c r="C171" t="s">
         <v>253</v>
       </c>
-      <c r="H171" s="27"/>
+      <c r="H171" s="36"/>
       <c r="L171" s="6"/>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.25">
@@ -3979,7 +4120,9 @@
       <c r="C175" t="s">
         <v>254</v>
       </c>
+      <c r="F175" s="26"/>
       <c r="H175" s="26"/>
+      <c r="J175" s="26"/>
       <c r="L175" s="6"/>
     </row>
     <row r="176" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3989,7 +4132,9 @@
       <c r="C176" t="s">
         <v>255</v>
       </c>
+      <c r="F176" s="26"/>
       <c r="H176" s="26"/>
+      <c r="J176" s="26"/>
       <c r="L176" s="6"/>
     </row>
     <row r="177" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>